<commit_message>
update manifest templates; bug fixes
</commit_message>
<xml_diff>
--- a/www/datasets_manifest.xlsx
+++ b/www/datasets_manifest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vchung/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2939F25D-0A96-A54E-8D43-E2C9259D2705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4DBC4D-452F-444F-8298-F1102784533F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8140" yWindow="460" windowWidth="20660" windowHeight="17540" xr2:uid="{CD4E31F0-ADA2-D447-8E73-A4C2A56D4DCF}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="standard_terms" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">standard_terms!$A$1:$C$415</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">standard_terms!$A$1:$C$417</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="447">
   <si>
     <t>datasetName</t>
   </si>
@@ -1373,6 +1373,12 @@
   </si>
   <si>
     <t>Leukemia</t>
+  </si>
+  <si>
+    <t>Hepatocellular Carcinoma</t>
+  </si>
+  <si>
+    <t>Breast Carcinoma</t>
   </si>
 </sst>
 </file>
@@ -1831,13 +1837,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Value is not one of the acceptable values for this column. Please see `standard_terms` tab for more information." prompt="Select value from the dropdown list." xr:uid="{C8BE928E-4EDA-7F43-A3FA-7A17BF6EF7A5}">
           <x14:formula1>
-            <xm:f>standard_terms!$B$157:$B$281</xm:f>
+            <xm:f>standard_terms!$B$157:$B$283</xm:f>
           </x14:formula1>
           <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Value is not one of the acceptable values for this column. Please see `standard_terms` tab for more information." prompt="Select value from the dropdown list." xr:uid="{432A9605-B035-F74B-9123-14AD720452A2}">
           <x14:formula1>
-            <xm:f>standard_terms!$B$282:$B$415</xm:f>
+            <xm:f>standard_terms!$B$284:$B$417</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
@@ -2019,7 +2025,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22616EE1-2275-CB41-A986-1AA97511F3EE}">
-  <dimension ref="A1:C415"/>
+  <dimension ref="A1:C417"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3954,7 +3960,7 @@
         <v>5</v>
       </c>
       <c r="B176" t="s">
-        <v>182</v>
+        <v>446</v>
       </c>
       <c r="C176" t="s">
         <v>442</v>
@@ -3965,7 +3971,7 @@
         <v>5</v>
       </c>
       <c r="B177" t="s">
-        <v>229</v>
+        <v>182</v>
       </c>
       <c r="C177" t="s">
         <v>442</v>
@@ -3976,7 +3982,7 @@
         <v>5</v>
       </c>
       <c r="B178" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="C178" t="s">
         <v>442</v>
@@ -3987,7 +3993,7 @@
         <v>5</v>
       </c>
       <c r="B179" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C179" t="s">
         <v>442</v>
@@ -3998,7 +4004,7 @@
         <v>5</v>
       </c>
       <c r="B180" t="s">
-        <v>170</v>
+        <v>210</v>
       </c>
       <c r="C180" t="s">
         <v>442</v>
@@ -4009,7 +4015,7 @@
         <v>5</v>
       </c>
       <c r="B181" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="C181" t="s">
         <v>442</v>
@@ -4020,7 +4026,7 @@
         <v>5</v>
       </c>
       <c r="B182" t="s">
-        <v>250</v>
+        <v>183</v>
       </c>
       <c r="C182" t="s">
         <v>442</v>
@@ -4031,7 +4037,7 @@
         <v>5</v>
       </c>
       <c r="B183" t="s">
-        <v>192</v>
+        <v>250</v>
       </c>
       <c r="C183" t="s">
         <v>442</v>
@@ -4042,7 +4048,7 @@
         <v>5</v>
       </c>
       <c r="B184" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C184" t="s">
         <v>442</v>
@@ -4053,7 +4059,7 @@
         <v>5</v>
       </c>
       <c r="B185" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="C185" t="s">
         <v>442</v>
@@ -4064,7 +4070,7 @@
         <v>5</v>
       </c>
       <c r="B186" t="s">
-        <v>271</v>
+        <v>214</v>
       </c>
       <c r="C186" t="s">
         <v>442</v>
@@ -4075,7 +4081,7 @@
         <v>5</v>
       </c>
       <c r="B187" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C187" t="s">
         <v>442</v>
@@ -4086,7 +4092,7 @@
         <v>5</v>
       </c>
       <c r="B188" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="C188" t="s">
         <v>442</v>
@@ -4097,7 +4103,7 @@
         <v>5</v>
       </c>
       <c r="B189" t="s">
-        <v>177</v>
+        <v>256</v>
       </c>
       <c r="C189" t="s">
         <v>442</v>
@@ -4108,7 +4114,7 @@
         <v>5</v>
       </c>
       <c r="B190" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="C190" t="s">
         <v>442</v>
@@ -4119,7 +4125,7 @@
         <v>5</v>
       </c>
       <c r="B191" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="C191" t="s">
         <v>442</v>
@@ -4130,7 +4136,7 @@
         <v>5</v>
       </c>
       <c r="B192" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C192" t="s">
         <v>442</v>
@@ -4141,7 +4147,7 @@
         <v>5</v>
       </c>
       <c r="B193" t="s">
-        <v>200</v>
+        <v>167</v>
       </c>
       <c r="C193" t="s">
         <v>442</v>
@@ -4152,7 +4158,7 @@
         <v>5</v>
       </c>
       <c r="B194" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="C194" t="s">
         <v>442</v>
@@ -4163,7 +4169,7 @@
         <v>5</v>
       </c>
       <c r="B195" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C195" t="s">
         <v>442</v>
@@ -4174,7 +4180,7 @@
         <v>5</v>
       </c>
       <c r="B196" t="s">
-        <v>428</v>
+        <v>231</v>
       </c>
       <c r="C196" t="s">
         <v>442</v>
@@ -4185,7 +4191,7 @@
         <v>5</v>
       </c>
       <c r="B197" t="s">
-        <v>196</v>
+        <v>428</v>
       </c>
       <c r="C197" t="s">
         <v>442</v>
@@ -4196,7 +4202,7 @@
         <v>5</v>
       </c>
       <c r="B198" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C198" t="s">
         <v>442</v>
@@ -4207,7 +4213,7 @@
         <v>5</v>
       </c>
       <c r="B199" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C199" t="s">
         <v>442</v>
@@ -4218,7 +4224,7 @@
         <v>5</v>
       </c>
       <c r="B200" t="s">
-        <v>443</v>
+        <v>198</v>
       </c>
       <c r="C200" t="s">
         <v>442</v>
@@ -4229,7 +4235,7 @@
         <v>5</v>
       </c>
       <c r="B201" t="s">
-        <v>199</v>
+        <v>443</v>
       </c>
       <c r="C201" t="s">
         <v>442</v>
@@ -4240,7 +4246,7 @@
         <v>5</v>
       </c>
       <c r="B202" t="s">
-        <v>232</v>
+        <v>199</v>
       </c>
       <c r="C202" t="s">
         <v>442</v>
@@ -4251,7 +4257,7 @@
         <v>5</v>
       </c>
       <c r="B203" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C203" t="s">
         <v>442</v>
@@ -4262,7 +4268,7 @@
         <v>5</v>
       </c>
       <c r="B204" t="s">
-        <v>430</v>
+        <v>275</v>
       </c>
       <c r="C204" t="s">
         <v>442</v>
@@ -4273,7 +4279,7 @@
         <v>5</v>
       </c>
       <c r="B205" t="s">
-        <v>281</v>
+        <v>430</v>
       </c>
       <c r="C205" t="s">
         <v>442</v>
@@ -4284,7 +4290,7 @@
         <v>5</v>
       </c>
       <c r="B206" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="C206" t="s">
         <v>442</v>
@@ -4295,7 +4301,7 @@
         <v>5</v>
       </c>
       <c r="B207" t="s">
-        <v>427</v>
+        <v>257</v>
       </c>
       <c r="C207" t="s">
         <v>442</v>
@@ -4306,7 +4312,7 @@
         <v>5</v>
       </c>
       <c r="B208" t="s">
-        <v>279</v>
+        <v>427</v>
       </c>
       <c r="C208" t="s">
         <v>442</v>
@@ -4317,7 +4323,7 @@
         <v>5</v>
       </c>
       <c r="B209" t="s">
-        <v>178</v>
+        <v>279</v>
       </c>
       <c r="C209" t="s">
         <v>442</v>
@@ -4328,7 +4334,7 @@
         <v>5</v>
       </c>
       <c r="B210" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C210" t="s">
         <v>442</v>
@@ -4339,7 +4345,7 @@
         <v>5</v>
       </c>
       <c r="B211" t="s">
-        <v>217</v>
+        <v>179</v>
       </c>
       <c r="C211" t="s">
         <v>442</v>
@@ -4350,7 +4356,7 @@
         <v>5</v>
       </c>
       <c r="B212" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C212" t="s">
         <v>442</v>
@@ -4361,7 +4367,7 @@
         <v>5</v>
       </c>
       <c r="B213" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C213" t="s">
         <v>442</v>
@@ -4372,7 +4378,7 @@
         <v>5</v>
       </c>
       <c r="B214" t="s">
-        <v>278</v>
+        <v>445</v>
       </c>
       <c r="C214" t="s">
         <v>442</v>
@@ -4383,7 +4389,7 @@
         <v>5</v>
       </c>
       <c r="B215" t="s">
-        <v>184</v>
+        <v>233</v>
       </c>
       <c r="C215" t="s">
         <v>442</v>
@@ -4394,7 +4400,7 @@
         <v>5</v>
       </c>
       <c r="B216" t="s">
-        <v>185</v>
+        <v>278</v>
       </c>
       <c r="C216" t="s">
         <v>442</v>
@@ -4405,7 +4411,7 @@
         <v>5</v>
       </c>
       <c r="B217" t="s">
-        <v>234</v>
+        <v>184</v>
       </c>
       <c r="C217" t="s">
         <v>442</v>
@@ -4416,7 +4422,7 @@
         <v>5</v>
       </c>
       <c r="B218" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="C218" t="s">
         <v>442</v>
@@ -4427,7 +4433,7 @@
         <v>5</v>
       </c>
       <c r="B219" t="s">
-        <v>444</v>
+        <v>234</v>
       </c>
       <c r="C219" t="s">
         <v>442</v>
@@ -4438,7 +4444,7 @@
         <v>5</v>
       </c>
       <c r="B220" t="s">
-        <v>248</v>
+        <v>201</v>
       </c>
       <c r="C220" t="s">
         <v>442</v>
@@ -4449,7 +4455,7 @@
         <v>5</v>
       </c>
       <c r="B221" t="s">
-        <v>249</v>
+        <v>444</v>
       </c>
       <c r="C221" t="s">
         <v>442</v>
@@ -4460,7 +4466,7 @@
         <v>5</v>
       </c>
       <c r="B222" t="s">
-        <v>186</v>
+        <v>248</v>
       </c>
       <c r="C222" t="s">
         <v>442</v>
@@ -4471,7 +4477,7 @@
         <v>5</v>
       </c>
       <c r="B223" t="s">
-        <v>187</v>
+        <v>249</v>
       </c>
       <c r="C223" t="s">
         <v>442</v>
@@ -4482,7 +4488,7 @@
         <v>5</v>
       </c>
       <c r="B224" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C224" t="s">
         <v>442</v>
@@ -4493,7 +4499,7 @@
         <v>5</v>
       </c>
       <c r="B225" t="s">
-        <v>251</v>
+        <v>187</v>
       </c>
       <c r="C225" t="s">
         <v>442</v>
@@ -4504,7 +4510,7 @@
         <v>5</v>
       </c>
       <c r="B226" t="s">
-        <v>252</v>
+        <v>188</v>
       </c>
       <c r="C226" t="s">
         <v>442</v>
@@ -4515,7 +4521,7 @@
         <v>5</v>
       </c>
       <c r="B227" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C227" t="s">
         <v>442</v>
@@ -4526,7 +4532,7 @@
         <v>5</v>
       </c>
       <c r="B228" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C228" t="s">
         <v>442</v>
@@ -4537,7 +4543,7 @@
         <v>5</v>
       </c>
       <c r="B229" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="C229" t="s">
         <v>442</v>
@@ -4548,7 +4554,7 @@
         <v>5</v>
       </c>
       <c r="B230" t="s">
-        <v>429</v>
+        <v>254</v>
       </c>
       <c r="C230" t="s">
         <v>442</v>
@@ -4559,7 +4565,7 @@
         <v>5</v>
       </c>
       <c r="B231" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C231" t="s">
         <v>442</v>
@@ -4570,7 +4576,7 @@
         <v>5</v>
       </c>
       <c r="B232" t="s">
-        <v>180</v>
+        <v>429</v>
       </c>
       <c r="C232" t="s">
         <v>442</v>
@@ -4581,7 +4587,7 @@
         <v>5</v>
       </c>
       <c r="B233" t="s">
-        <v>262</v>
+        <v>236</v>
       </c>
       <c r="C233" t="s">
         <v>442</v>
@@ -4592,7 +4598,7 @@
         <v>5</v>
       </c>
       <c r="B234" t="s">
-        <v>264</v>
+        <v>180</v>
       </c>
       <c r="C234" t="s">
         <v>442</v>
@@ -4603,7 +4609,7 @@
         <v>5</v>
       </c>
       <c r="B235" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C235" t="s">
         <v>442</v>
@@ -4614,7 +4620,7 @@
         <v>5</v>
       </c>
       <c r="B236" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C236" t="s">
         <v>442</v>
@@ -4625,7 +4631,7 @@
         <v>5</v>
       </c>
       <c r="B237" t="s">
-        <v>237</v>
+        <v>258</v>
       </c>
       <c r="C237" t="s">
         <v>442</v>
@@ -4636,7 +4642,7 @@
         <v>5</v>
       </c>
       <c r="B238" t="s">
-        <v>238</v>
+        <v>259</v>
       </c>
       <c r="C238" t="s">
         <v>442</v>
@@ -4647,7 +4653,7 @@
         <v>5</v>
       </c>
       <c r="B239" t="s">
-        <v>181</v>
+        <v>237</v>
       </c>
       <c r="C239" t="s">
         <v>442</v>
@@ -4658,7 +4664,7 @@
         <v>5</v>
       </c>
       <c r="B240" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="C240" t="s">
         <v>442</v>
@@ -4669,7 +4675,7 @@
         <v>5</v>
       </c>
       <c r="B241" t="s">
-        <v>239</v>
+        <v>181</v>
       </c>
       <c r="C241" t="s">
         <v>442</v>
@@ -4680,7 +4686,7 @@
         <v>5</v>
       </c>
       <c r="B242" t="s">
-        <v>219</v>
+        <v>276</v>
       </c>
       <c r="C242" t="s">
         <v>442</v>
@@ -4691,7 +4697,7 @@
         <v>5</v>
       </c>
       <c r="B243" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C243" t="s">
         <v>442</v>
@@ -4702,7 +4708,7 @@
         <v>5</v>
       </c>
       <c r="B244" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="C244" t="s">
         <v>442</v>
@@ -4713,7 +4719,7 @@
         <v>5</v>
       </c>
       <c r="B245" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C245" t="s">
         <v>442</v>
@@ -4724,7 +4730,7 @@
         <v>5</v>
       </c>
       <c r="B246" t="s">
-        <v>202</v>
+        <v>241</v>
       </c>
       <c r="C246" t="s">
         <v>442</v>
@@ -4735,7 +4741,7 @@
         <v>5</v>
       </c>
       <c r="B247" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="C247" t="s">
         <v>442</v>
@@ -4746,7 +4752,7 @@
         <v>5</v>
       </c>
       <c r="B248" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C248" t="s">
         <v>442</v>
@@ -4757,7 +4763,7 @@
         <v>5</v>
       </c>
       <c r="B249" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C249" t="s">
         <v>442</v>
@@ -4768,7 +4774,7 @@
         <v>5</v>
       </c>
       <c r="B250" t="s">
-        <v>243</v>
+        <v>211</v>
       </c>
       <c r="C250" t="s">
         <v>442</v>
@@ -4779,7 +4785,7 @@
         <v>5</v>
       </c>
       <c r="B251" t="s">
-        <v>220</v>
+        <v>270</v>
       </c>
       <c r="C251" t="s">
         <v>442</v>
@@ -4790,7 +4796,7 @@
         <v>5</v>
       </c>
       <c r="B252" t="s">
-        <v>221</v>
+        <v>243</v>
       </c>
       <c r="C252" t="s">
         <v>442</v>
@@ -4801,7 +4807,7 @@
         <v>5</v>
       </c>
       <c r="B253" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="C253" t="s">
         <v>442</v>
@@ -4812,7 +4818,7 @@
         <v>5</v>
       </c>
       <c r="B254" t="s">
-        <v>263</v>
+        <v>221</v>
       </c>
       <c r="C254" t="s">
         <v>442</v>
@@ -4823,7 +4829,7 @@
         <v>5</v>
       </c>
       <c r="B255" t="s">
-        <v>265</v>
+        <v>203</v>
       </c>
       <c r="C255" t="s">
         <v>442</v>
@@ -4834,7 +4840,7 @@
         <v>5</v>
       </c>
       <c r="B256" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C256" t="s">
         <v>442</v>
@@ -4845,7 +4851,7 @@
         <v>5</v>
       </c>
       <c r="B257" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C257" t="s">
         <v>442</v>
@@ -4856,7 +4862,7 @@
         <v>5</v>
       </c>
       <c r="B258" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C258" t="s">
         <v>442</v>
@@ -4867,7 +4873,7 @@
         <v>5</v>
       </c>
       <c r="B259" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C259" t="s">
         <v>442</v>
@@ -4878,7 +4884,7 @@
         <v>5</v>
       </c>
       <c r="B260" t="s">
-        <v>189</v>
+        <v>268</v>
       </c>
       <c r="C260" t="s">
         <v>442</v>
@@ -4889,7 +4895,7 @@
         <v>5</v>
       </c>
       <c r="B261" t="s">
-        <v>223</v>
+        <v>269</v>
       </c>
       <c r="C261" t="s">
         <v>442</v>
@@ -4900,7 +4906,7 @@
         <v>5</v>
       </c>
       <c r="B262" t="s">
-        <v>244</v>
+        <v>189</v>
       </c>
       <c r="C262" t="s">
         <v>442</v>
@@ -4911,7 +4917,7 @@
         <v>5</v>
       </c>
       <c r="B263" t="s">
-        <v>272</v>
+        <v>223</v>
       </c>
       <c r="C263" t="s">
         <v>442</v>
@@ -4922,7 +4928,7 @@
         <v>5</v>
       </c>
       <c r="B264" t="s">
-        <v>273</v>
+        <v>244</v>
       </c>
       <c r="C264" t="s">
         <v>442</v>
@@ -4933,7 +4939,7 @@
         <v>5</v>
       </c>
       <c r="B265" t="s">
-        <v>172</v>
+        <v>272</v>
       </c>
       <c r="C265" t="s">
         <v>442</v>
@@ -4944,7 +4950,7 @@
         <v>5</v>
       </c>
       <c r="B266" t="s">
-        <v>247</v>
+        <v>273</v>
       </c>
       <c r="C266" t="s">
         <v>442</v>
@@ -4955,7 +4961,7 @@
         <v>5</v>
       </c>
       <c r="B267" t="s">
-        <v>205</v>
+        <v>172</v>
       </c>
       <c r="C267" t="s">
         <v>442</v>
@@ -4966,7 +4972,7 @@
         <v>5</v>
       </c>
       <c r="B268" t="s">
-        <v>204</v>
+        <v>247</v>
       </c>
       <c r="C268" t="s">
         <v>442</v>
@@ -4977,7 +4983,7 @@
         <v>5</v>
       </c>
       <c r="B269" t="s">
-        <v>277</v>
+        <v>205</v>
       </c>
       <c r="C269" t="s">
         <v>442</v>
@@ -4988,7 +4994,7 @@
         <v>5</v>
       </c>
       <c r="B270" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="C270" t="s">
         <v>442</v>
@@ -4999,7 +5005,7 @@
         <v>5</v>
       </c>
       <c r="B271" t="s">
-        <v>212</v>
+        <v>277</v>
       </c>
       <c r="C271" t="s">
         <v>442</v>
@@ -5010,7 +5016,7 @@
         <v>5</v>
       </c>
       <c r="B272" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C272" t="s">
         <v>442</v>
@@ -5021,7 +5027,7 @@
         <v>5</v>
       </c>
       <c r="B273" t="s">
-        <v>280</v>
+        <v>212</v>
       </c>
       <c r="C273" t="s">
         <v>442</v>
@@ -5032,7 +5038,7 @@
         <v>5</v>
       </c>
       <c r="B274" t="s">
-        <v>173</v>
+        <v>222</v>
       </c>
       <c r="C274" t="s">
         <v>442</v>
@@ -5043,7 +5049,7 @@
         <v>5</v>
       </c>
       <c r="B275" t="s">
-        <v>245</v>
+        <v>280</v>
       </c>
       <c r="C275" t="s">
         <v>442</v>
@@ -5054,7 +5060,7 @@
         <v>5</v>
       </c>
       <c r="B276" t="s">
-        <v>246</v>
+        <v>173</v>
       </c>
       <c r="C276" t="s">
         <v>442</v>
@@ -5065,7 +5071,7 @@
         <v>5</v>
       </c>
       <c r="B277" t="s">
-        <v>190</v>
+        <v>245</v>
       </c>
       <c r="C277" t="s">
         <v>442</v>
@@ -5076,7 +5082,7 @@
         <v>5</v>
       </c>
       <c r="B278" t="s">
-        <v>191</v>
+        <v>246</v>
       </c>
       <c r="C278" t="s">
         <v>442</v>
@@ -5087,7 +5093,7 @@
         <v>5</v>
       </c>
       <c r="B279" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C279" t="s">
         <v>442</v>
@@ -5098,7 +5104,7 @@
         <v>5</v>
       </c>
       <c r="B280" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="C280" t="s">
         <v>442</v>
@@ -5109,7 +5115,7 @@
         <v>5</v>
       </c>
       <c r="B281" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="C281" t="s">
         <v>442</v>
@@ -5117,7 +5123,10 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A282" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B282" t="s">
+        <v>215</v>
       </c>
       <c r="C282" t="s">
         <v>442</v>
@@ -5125,10 +5134,10 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A283" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B283" t="s">
-        <v>363</v>
+        <v>216</v>
       </c>
       <c r="C283" t="s">
         <v>442</v>
@@ -5138,9 +5147,6 @@
       <c r="A284" t="s">
         <v>6</v>
       </c>
-      <c r="B284" t="s">
-        <v>306</v>
-      </c>
       <c r="C284" t="s">
         <v>442</v>
       </c>
@@ -5150,7 +5156,7 @@
         <v>6</v>
       </c>
       <c r="B285" t="s">
-        <v>385</v>
+        <v>363</v>
       </c>
       <c r="C285" t="s">
         <v>442</v>
@@ -5161,7 +5167,7 @@
         <v>6</v>
       </c>
       <c r="B286" t="s">
-        <v>384</v>
+        <v>306</v>
       </c>
       <c r="C286" t="s">
         <v>442</v>
@@ -5172,7 +5178,7 @@
         <v>6</v>
       </c>
       <c r="B287" t="s">
-        <v>336</v>
+        <v>385</v>
       </c>
       <c r="C287" t="s">
         <v>442</v>
@@ -5183,7 +5189,7 @@
         <v>6</v>
       </c>
       <c r="B288" t="s">
-        <v>337</v>
+        <v>384</v>
       </c>
       <c r="C288" t="s">
         <v>442</v>
@@ -5194,7 +5200,7 @@
         <v>6</v>
       </c>
       <c r="B289" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="C289" t="s">
         <v>442</v>
@@ -5205,7 +5211,7 @@
         <v>6</v>
       </c>
       <c r="B290" t="s">
-        <v>390</v>
+        <v>337</v>
       </c>
       <c r="C290" t="s">
         <v>442</v>
@@ -5216,7 +5222,7 @@
         <v>6</v>
       </c>
       <c r="B291" t="s">
-        <v>425</v>
+        <v>332</v>
       </c>
       <c r="C291" t="s">
         <v>442</v>
@@ -5227,7 +5233,7 @@
         <v>6</v>
       </c>
       <c r="B292" t="s">
-        <v>320</v>
+        <v>390</v>
       </c>
       <c r="C292" t="s">
         <v>442</v>
@@ -5238,7 +5244,7 @@
         <v>6</v>
       </c>
       <c r="B293" t="s">
-        <v>354</v>
+        <v>425</v>
       </c>
       <c r="C293" t="s">
         <v>442</v>
@@ -5249,7 +5255,7 @@
         <v>6</v>
       </c>
       <c r="B294" t="s">
-        <v>371</v>
+        <v>320</v>
       </c>
       <c r="C294" t="s">
         <v>442</v>
@@ -5260,7 +5266,7 @@
         <v>6</v>
       </c>
       <c r="B295" t="s">
-        <v>398</v>
+        <v>354</v>
       </c>
       <c r="C295" t="s">
         <v>442</v>
@@ -5271,7 +5277,7 @@
         <v>6</v>
       </c>
       <c r="B296" t="s">
-        <v>321</v>
+        <v>371</v>
       </c>
       <c r="C296" t="s">
         <v>442</v>
@@ -5282,7 +5288,7 @@
         <v>6</v>
       </c>
       <c r="B297" t="s">
-        <v>310</v>
+        <v>398</v>
       </c>
       <c r="C297" t="s">
         <v>442</v>
@@ -5293,7 +5299,7 @@
         <v>6</v>
       </c>
       <c r="B298" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C298" t="s">
         <v>442</v>
@@ -5304,7 +5310,7 @@
         <v>6</v>
       </c>
       <c r="B299" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="C299" t="s">
         <v>442</v>
@@ -5315,7 +5321,7 @@
         <v>6</v>
       </c>
       <c r="B300" t="s">
-        <v>369</v>
+        <v>317</v>
       </c>
       <c r="C300" t="s">
         <v>442</v>
@@ -5326,7 +5332,7 @@
         <v>6</v>
       </c>
       <c r="B301" t="s">
-        <v>303</v>
+        <v>325</v>
       </c>
       <c r="C301" t="s">
         <v>442</v>
@@ -5337,7 +5343,7 @@
         <v>6</v>
       </c>
       <c r="B302" t="s">
-        <v>335</v>
+        <v>369</v>
       </c>
       <c r="C302" t="s">
         <v>442</v>
@@ -5348,7 +5354,7 @@
         <v>6</v>
       </c>
       <c r="B303" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
       <c r="C303" t="s">
         <v>442</v>
@@ -5359,7 +5365,7 @@
         <v>6</v>
       </c>
       <c r="B304" t="s">
-        <v>316</v>
+        <v>335</v>
       </c>
       <c r="C304" t="s">
         <v>442</v>
@@ -5370,7 +5376,7 @@
         <v>6</v>
       </c>
       <c r="B305" t="s">
-        <v>311</v>
+        <v>327</v>
       </c>
       <c r="C305" t="s">
         <v>442</v>
@@ -5381,7 +5387,7 @@
         <v>6</v>
       </c>
       <c r="B306" t="s">
-        <v>361</v>
+        <v>316</v>
       </c>
       <c r="C306" t="s">
         <v>442</v>
@@ -5392,7 +5398,7 @@
         <v>6</v>
       </c>
       <c r="B307" t="s">
-        <v>399</v>
+        <v>311</v>
       </c>
       <c r="C307" t="s">
         <v>442</v>
@@ -5403,7 +5409,7 @@
         <v>6</v>
       </c>
       <c r="B308" t="s">
-        <v>386</v>
+        <v>361</v>
       </c>
       <c r="C308" t="s">
         <v>442</v>
@@ -5414,7 +5420,7 @@
         <v>6</v>
       </c>
       <c r="B309" t="s">
-        <v>334</v>
+        <v>399</v>
       </c>
       <c r="C309" t="s">
         <v>442</v>
@@ -5425,7 +5431,7 @@
         <v>6</v>
       </c>
       <c r="B310" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="C310" t="s">
         <v>442</v>
@@ -5436,7 +5442,7 @@
         <v>6</v>
       </c>
       <c r="B311" t="s">
-        <v>307</v>
+        <v>334</v>
       </c>
       <c r="C311" t="s">
         <v>442</v>
@@ -5447,7 +5453,7 @@
         <v>6</v>
       </c>
       <c r="B312" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="C312" t="s">
         <v>442</v>
@@ -5458,7 +5464,7 @@
         <v>6</v>
       </c>
       <c r="B313" t="s">
-        <v>341</v>
+        <v>307</v>
       </c>
       <c r="C313" t="s">
         <v>442</v>
@@ -5469,7 +5475,7 @@
         <v>6</v>
       </c>
       <c r="B314" t="s">
-        <v>378</v>
+        <v>407</v>
       </c>
       <c r="C314" t="s">
         <v>442</v>
@@ -5480,7 +5486,7 @@
         <v>6</v>
       </c>
       <c r="B315" t="s">
-        <v>409</v>
+        <v>341</v>
       </c>
       <c r="C315" t="s">
         <v>442</v>
@@ -5491,7 +5497,7 @@
         <v>6</v>
       </c>
       <c r="B316" t="s">
-        <v>408</v>
+        <v>378</v>
       </c>
       <c r="C316" t="s">
         <v>442</v>
@@ -5502,7 +5508,7 @@
         <v>6</v>
       </c>
       <c r="B317" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="C317" t="s">
         <v>442</v>
@@ -5513,7 +5519,7 @@
         <v>6</v>
       </c>
       <c r="B318" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C318" t="s">
         <v>442</v>
@@ -5524,7 +5530,7 @@
         <v>6</v>
       </c>
       <c r="B319" t="s">
-        <v>360</v>
+        <v>400</v>
       </c>
       <c r="C319" t="s">
         <v>442</v>
@@ -5535,7 +5541,7 @@
         <v>6</v>
       </c>
       <c r="B320" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="C320" t="s">
         <v>442</v>
@@ -5546,7 +5552,7 @@
         <v>6</v>
       </c>
       <c r="B321" t="s">
-        <v>295</v>
+        <v>360</v>
       </c>
       <c r="C321" t="s">
         <v>442</v>
@@ -5557,7 +5563,7 @@
         <v>6</v>
       </c>
       <c r="B322" t="s">
-        <v>293</v>
+        <v>401</v>
       </c>
       <c r="C322" t="s">
         <v>442</v>
@@ -5568,7 +5574,7 @@
         <v>6</v>
       </c>
       <c r="B323" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C323" t="s">
         <v>442</v>
@@ -5579,7 +5585,7 @@
         <v>6</v>
       </c>
       <c r="B324" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
       <c r="C324" t="s">
         <v>442</v>
@@ -5590,7 +5596,7 @@
         <v>6</v>
       </c>
       <c r="B325" t="s">
-        <v>370</v>
+        <v>294</v>
       </c>
       <c r="C325" t="s">
         <v>442</v>
@@ -5601,7 +5607,7 @@
         <v>6</v>
       </c>
       <c r="B326" t="s">
-        <v>391</v>
+        <v>319</v>
       </c>
       <c r="C326" t="s">
         <v>442</v>
@@ -5612,7 +5618,7 @@
         <v>6</v>
       </c>
       <c r="B327" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C327" t="s">
         <v>442</v>
@@ -5623,7 +5629,7 @@
         <v>6</v>
       </c>
       <c r="B328" t="s">
-        <v>375</v>
+        <v>391</v>
       </c>
       <c r="C328" t="s">
         <v>442</v>
@@ -5634,7 +5640,7 @@
         <v>6</v>
       </c>
       <c r="B329" t="s">
-        <v>292</v>
+        <v>372</v>
       </c>
       <c r="C329" t="s">
         <v>442</v>
@@ -5645,7 +5651,7 @@
         <v>6</v>
       </c>
       <c r="B330" t="s">
-        <v>353</v>
+        <v>375</v>
       </c>
       <c r="C330" t="s">
         <v>442</v>
@@ -5656,7 +5662,7 @@
         <v>6</v>
       </c>
       <c r="B331" t="s">
-        <v>324</v>
+        <v>292</v>
       </c>
       <c r="C331" t="s">
         <v>442</v>
@@ -5667,7 +5673,7 @@
         <v>6</v>
       </c>
       <c r="B332" t="s">
-        <v>338</v>
+        <v>353</v>
       </c>
       <c r="C332" t="s">
         <v>442</v>
@@ -5678,7 +5684,7 @@
         <v>6</v>
       </c>
       <c r="B333" t="s">
-        <v>380</v>
+        <v>324</v>
       </c>
       <c r="C333" t="s">
         <v>442</v>
@@ -5689,7 +5695,7 @@
         <v>6</v>
       </c>
       <c r="B334" t="s">
-        <v>286</v>
+        <v>338</v>
       </c>
       <c r="C334" t="s">
         <v>442</v>
@@ -5700,7 +5706,7 @@
         <v>6</v>
       </c>
       <c r="B335" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="C335" t="s">
         <v>442</v>
@@ -5711,7 +5717,7 @@
         <v>6</v>
       </c>
       <c r="B336" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C336" t="s">
         <v>442</v>
@@ -5722,7 +5728,7 @@
         <v>6</v>
       </c>
       <c r="B337" t="s">
-        <v>357</v>
+        <v>389</v>
       </c>
       <c r="C337" t="s">
         <v>442</v>
@@ -5733,7 +5739,7 @@
         <v>6</v>
       </c>
       <c r="B338" t="s">
-        <v>379</v>
+        <v>285</v>
       </c>
       <c r="C338" t="s">
         <v>442</v>
@@ -5744,7 +5750,7 @@
         <v>6</v>
       </c>
       <c r="B339" t="s">
-        <v>290</v>
+        <v>357</v>
       </c>
       <c r="C339" t="s">
         <v>442</v>
@@ -5755,7 +5761,7 @@
         <v>6</v>
       </c>
       <c r="B340" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="C340" t="s">
         <v>442</v>
@@ -5766,7 +5772,7 @@
         <v>6</v>
       </c>
       <c r="B341" t="s">
-        <v>388</v>
+        <v>290</v>
       </c>
       <c r="C341" t="s">
         <v>442</v>
@@ -5777,7 +5783,7 @@
         <v>6</v>
       </c>
       <c r="B342" t="s">
-        <v>348</v>
+        <v>374</v>
       </c>
       <c r="C342" t="s">
         <v>442</v>
@@ -5788,7 +5794,7 @@
         <v>6</v>
       </c>
       <c r="B343" t="s">
-        <v>366</v>
+        <v>388</v>
       </c>
       <c r="C343" t="s">
         <v>442</v>
@@ -5799,7 +5805,7 @@
         <v>6</v>
       </c>
       <c r="B344" t="s">
-        <v>329</v>
+        <v>348</v>
       </c>
       <c r="C344" t="s">
         <v>442</v>
@@ -5810,7 +5816,7 @@
         <v>6</v>
       </c>
       <c r="B345" t="s">
-        <v>331</v>
+        <v>366</v>
       </c>
       <c r="C345" t="s">
         <v>442</v>
@@ -5821,7 +5827,7 @@
         <v>6</v>
       </c>
       <c r="B346" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="C346" t="s">
         <v>442</v>
@@ -5832,7 +5838,7 @@
         <v>6</v>
       </c>
       <c r="B347" t="s">
-        <v>282</v>
+        <v>331</v>
       </c>
       <c r="C347" t="s">
         <v>442</v>
@@ -5843,7 +5849,7 @@
         <v>6</v>
       </c>
       <c r="B348" t="s">
-        <v>287</v>
+        <v>344</v>
       </c>
       <c r="C348" t="s">
         <v>442</v>
@@ -5854,7 +5860,7 @@
         <v>6</v>
       </c>
       <c r="B349" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C349" t="s">
         <v>442</v>
@@ -5865,7 +5871,7 @@
         <v>6</v>
       </c>
       <c r="B350" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C350" t="s">
         <v>442</v>
@@ -5876,7 +5882,7 @@
         <v>6</v>
       </c>
       <c r="B351" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C351" t="s">
         <v>442</v>
@@ -5887,7 +5893,7 @@
         <v>6</v>
       </c>
       <c r="B352" t="s">
-        <v>345</v>
+        <v>288</v>
       </c>
       <c r="C352" t="s">
         <v>442</v>
@@ -5898,7 +5904,7 @@
         <v>6</v>
       </c>
       <c r="B353" t="s">
-        <v>410</v>
+        <v>283</v>
       </c>
       <c r="C353" t="s">
         <v>442</v>
@@ -5909,7 +5915,7 @@
         <v>6</v>
       </c>
       <c r="B354" t="s">
-        <v>381</v>
+        <v>345</v>
       </c>
       <c r="C354" t="s">
         <v>442</v>
@@ -5920,7 +5926,7 @@
         <v>6</v>
       </c>
       <c r="B355" t="s">
-        <v>393</v>
+        <v>410</v>
       </c>
       <c r="C355" t="s">
         <v>442</v>
@@ -5931,7 +5937,7 @@
         <v>6</v>
       </c>
       <c r="B356" t="s">
-        <v>347</v>
+        <v>381</v>
       </c>
       <c r="C356" t="s">
         <v>442</v>
@@ -5942,7 +5948,7 @@
         <v>6</v>
       </c>
       <c r="B357" t="s">
-        <v>365</v>
+        <v>393</v>
       </c>
       <c r="C357" t="s">
         <v>442</v>
@@ -5953,7 +5959,7 @@
         <v>6</v>
       </c>
       <c r="B358" t="s">
-        <v>395</v>
+        <v>347</v>
       </c>
       <c r="C358" t="s">
         <v>442</v>
@@ -5964,7 +5970,7 @@
         <v>6</v>
       </c>
       <c r="B359" t="s">
-        <v>392</v>
+        <v>365</v>
       </c>
       <c r="C359" t="s">
         <v>442</v>
@@ -5975,7 +5981,7 @@
         <v>6</v>
       </c>
       <c r="B360" t="s">
-        <v>301</v>
+        <v>395</v>
       </c>
       <c r="C360" t="s">
         <v>442</v>
@@ -5986,7 +5992,7 @@
         <v>6</v>
       </c>
       <c r="B361" t="s">
-        <v>326</v>
+        <v>392</v>
       </c>
       <c r="C361" t="s">
         <v>442</v>
@@ -5997,7 +6003,7 @@
         <v>6</v>
       </c>
       <c r="B362" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="C362" t="s">
         <v>442</v>
@@ -6008,7 +6014,7 @@
         <v>6</v>
       </c>
       <c r="B363" t="s">
-        <v>304</v>
+        <v>326</v>
       </c>
       <c r="C363" t="s">
         <v>442</v>
@@ -6019,7 +6025,7 @@
         <v>6</v>
       </c>
       <c r="B364" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C364" t="s">
         <v>442</v>
@@ -6030,7 +6036,7 @@
         <v>6</v>
       </c>
       <c r="B365" t="s">
-        <v>359</v>
+        <v>304</v>
       </c>
       <c r="C365" t="s">
         <v>442</v>
@@ -6041,7 +6047,7 @@
         <v>6</v>
       </c>
       <c r="B366" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="C366" t="s">
         <v>442</v>
@@ -6052,7 +6058,7 @@
         <v>6</v>
       </c>
       <c r="B367" t="s">
-        <v>308</v>
+        <v>359</v>
       </c>
       <c r="C367" t="s">
         <v>442</v>
@@ -6063,7 +6069,7 @@
         <v>6</v>
       </c>
       <c r="B368" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="C368" t="s">
         <v>442</v>
@@ -6074,7 +6080,7 @@
         <v>6</v>
       </c>
       <c r="B369" t="s">
-        <v>402</v>
+        <v>308</v>
       </c>
       <c r="C369" t="s">
         <v>442</v>
@@ -6085,7 +6091,7 @@
         <v>6</v>
       </c>
       <c r="B370" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="C370" t="s">
         <v>442</v>
@@ -6096,7 +6102,7 @@
         <v>6</v>
       </c>
       <c r="B371" t="s">
-        <v>367</v>
+        <v>402</v>
       </c>
       <c r="C371" t="s">
         <v>442</v>
@@ -6107,7 +6113,7 @@
         <v>6</v>
       </c>
       <c r="B372" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C372" t="s">
         <v>442</v>
@@ -6118,7 +6124,7 @@
         <v>6</v>
       </c>
       <c r="B373" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="C373" t="s">
         <v>442</v>
@@ -6129,7 +6135,7 @@
         <v>6</v>
       </c>
       <c r="B374" t="s">
-        <v>387</v>
+        <v>349</v>
       </c>
       <c r="C374" t="s">
         <v>442</v>
@@ -6140,7 +6146,7 @@
         <v>6</v>
       </c>
       <c r="B375" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
       <c r="C375" t="s">
         <v>442</v>
@@ -6151,7 +6157,7 @@
         <v>6</v>
       </c>
       <c r="B376" t="s">
-        <v>376</v>
+        <v>387</v>
       </c>
       <c r="C376" t="s">
         <v>442</v>
@@ -6162,7 +6168,7 @@
         <v>6</v>
       </c>
       <c r="B377" t="s">
-        <v>352</v>
+        <v>382</v>
       </c>
       <c r="C377" t="s">
         <v>442</v>
@@ -6173,7 +6179,7 @@
         <v>6</v>
       </c>
       <c r="B378" t="s">
-        <v>356</v>
+        <v>376</v>
       </c>
       <c r="C378" t="s">
         <v>442</v>
@@ -6184,7 +6190,7 @@
         <v>6</v>
       </c>
       <c r="B379" t="s">
-        <v>313</v>
+        <v>352</v>
       </c>
       <c r="C379" t="s">
         <v>442</v>
@@ -6195,7 +6201,7 @@
         <v>6</v>
       </c>
       <c r="B380" t="s">
-        <v>289</v>
+        <v>356</v>
       </c>
       <c r="C380" t="s">
         <v>442</v>
@@ -6206,7 +6212,7 @@
         <v>6</v>
       </c>
       <c r="B381" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C381" t="s">
         <v>442</v>
@@ -6217,7 +6223,7 @@
         <v>6</v>
       </c>
       <c r="B382" t="s">
-        <v>351</v>
+        <v>289</v>
       </c>
       <c r="C382" t="s">
         <v>442</v>
@@ -6228,7 +6234,7 @@
         <v>6</v>
       </c>
       <c r="B383" t="s">
-        <v>373</v>
+        <v>309</v>
       </c>
       <c r="C383" t="s">
         <v>442</v>
@@ -6239,7 +6245,7 @@
         <v>6</v>
       </c>
       <c r="B384" t="s">
-        <v>383</v>
+        <v>351</v>
       </c>
       <c r="C384" t="s">
         <v>442</v>
@@ -6250,7 +6256,7 @@
         <v>6</v>
       </c>
       <c r="B385" t="s">
-        <v>323</v>
+        <v>373</v>
       </c>
       <c r="C385" t="s">
         <v>442</v>
@@ -6261,7 +6267,7 @@
         <v>6</v>
       </c>
       <c r="B386" t="s">
-        <v>342</v>
+        <v>383</v>
       </c>
       <c r="C386" t="s">
         <v>442</v>
@@ -6272,7 +6278,7 @@
         <v>6</v>
       </c>
       <c r="B387" t="s">
-        <v>291</v>
+        <v>323</v>
       </c>
       <c r="C387" t="s">
         <v>442</v>
@@ -6283,7 +6289,7 @@
         <v>6</v>
       </c>
       <c r="B388" t="s">
-        <v>299</v>
+        <v>342</v>
       </c>
       <c r="C388" t="s">
         <v>442</v>
@@ -6294,7 +6300,7 @@
         <v>6</v>
       </c>
       <c r="B389" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C389" t="s">
         <v>442</v>
@@ -6305,7 +6311,7 @@
         <v>6</v>
       </c>
       <c r="B390" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C390" t="s">
         <v>442</v>
@@ -6316,7 +6322,7 @@
         <v>6</v>
       </c>
       <c r="B391" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C391" t="s">
         <v>442</v>
@@ -6327,7 +6333,7 @@
         <v>6</v>
       </c>
       <c r="B392" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C392" t="s">
         <v>442</v>
@@ -6338,7 +6344,7 @@
         <v>6</v>
       </c>
       <c r="B393" t="s">
-        <v>377</v>
+        <v>297</v>
       </c>
       <c r="C393" t="s">
         <v>442</v>
@@ -6349,7 +6355,7 @@
         <v>6</v>
       </c>
       <c r="B394" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C394" t="s">
         <v>442</v>
@@ -6360,7 +6366,7 @@
         <v>6</v>
       </c>
       <c r="B395" t="s">
-        <v>322</v>
+        <v>377</v>
       </c>
       <c r="C395" t="s">
         <v>442</v>
@@ -6371,7 +6377,7 @@
         <v>6</v>
       </c>
       <c r="B396" t="s">
-        <v>340</v>
+        <v>302</v>
       </c>
       <c r="C396" t="s">
         <v>442</v>
@@ -6382,7 +6388,7 @@
         <v>6</v>
       </c>
       <c r="B397" t="s">
-        <v>368</v>
+        <v>322</v>
       </c>
       <c r="C397" t="s">
         <v>442</v>
@@ -6393,7 +6399,7 @@
         <v>6</v>
       </c>
       <c r="B398" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="C398" t="s">
         <v>442</v>
@@ -6404,7 +6410,7 @@
         <v>6</v>
       </c>
       <c r="B399" t="s">
-        <v>312</v>
+        <v>368</v>
       </c>
       <c r="C399" t="s">
         <v>442</v>
@@ -6415,7 +6421,7 @@
         <v>6</v>
       </c>
       <c r="B400" t="s">
-        <v>405</v>
+        <v>355</v>
       </c>
       <c r="C400" t="s">
         <v>442</v>
@@ -6426,7 +6432,7 @@
         <v>6</v>
       </c>
       <c r="B401" t="s">
-        <v>362</v>
+        <v>312</v>
       </c>
       <c r="C401" t="s">
         <v>442</v>
@@ -6437,7 +6443,7 @@
         <v>6</v>
       </c>
       <c r="B402" t="s">
-        <v>394</v>
+        <v>405</v>
       </c>
       <c r="C402" t="s">
         <v>442</v>
@@ -6448,7 +6454,7 @@
         <v>6</v>
       </c>
       <c r="B403" t="s">
-        <v>426</v>
+        <v>362</v>
       </c>
       <c r="C403" t="s">
         <v>442</v>
@@ -6459,7 +6465,7 @@
         <v>6</v>
       </c>
       <c r="B404" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C404" t="s">
         <v>442</v>
@@ -6470,7 +6476,7 @@
         <v>6</v>
       </c>
       <c r="B405" t="s">
-        <v>350</v>
+        <v>426</v>
       </c>
       <c r="C405" t="s">
         <v>442</v>
@@ -6481,7 +6487,7 @@
         <v>6</v>
       </c>
       <c r="B406" t="s">
-        <v>339</v>
+        <v>396</v>
       </c>
       <c r="C406" t="s">
         <v>442</v>
@@ -6492,7 +6498,7 @@
         <v>6</v>
       </c>
       <c r="B407" t="s">
-        <v>406</v>
+        <v>350</v>
       </c>
       <c r="C407" t="s">
         <v>442</v>
@@ -6503,7 +6509,7 @@
         <v>6</v>
       </c>
       <c r="B408" t="s">
-        <v>150</v>
+        <v>339</v>
       </c>
       <c r="C408" t="s">
         <v>442</v>
@@ -6514,7 +6520,7 @@
         <v>6</v>
       </c>
       <c r="B409" t="s">
-        <v>346</v>
+        <v>406</v>
       </c>
       <c r="C409" t="s">
         <v>442</v>
@@ -6525,7 +6531,7 @@
         <v>6</v>
       </c>
       <c r="B410" t="s">
-        <v>364</v>
+        <v>150</v>
       </c>
       <c r="C410" t="s">
         <v>442</v>
@@ -6536,7 +6542,7 @@
         <v>6</v>
       </c>
       <c r="B411" t="s">
-        <v>328</v>
+        <v>346</v>
       </c>
       <c r="C411" t="s">
         <v>442</v>
@@ -6547,7 +6553,7 @@
         <v>6</v>
       </c>
       <c r="B412" t="s">
-        <v>330</v>
+        <v>364</v>
       </c>
       <c r="C412" t="s">
         <v>442</v>
@@ -6558,7 +6564,7 @@
         <v>6</v>
       </c>
       <c r="B413" t="s">
-        <v>404</v>
+        <v>328</v>
       </c>
       <c r="C413" t="s">
         <v>442</v>
@@ -6569,7 +6575,7 @@
         <v>6</v>
       </c>
       <c r="B414" t="s">
-        <v>403</v>
+        <v>330</v>
       </c>
       <c r="C414" t="s">
         <v>442</v>
@@ -6580,17 +6586,39 @@
         <v>6</v>
       </c>
       <c r="B415" t="s">
+        <v>404</v>
+      </c>
+      <c r="C415" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A416" t="s">
+        <v>6</v>
+      </c>
+      <c r="B416" t="s">
+        <v>403</v>
+      </c>
+      <c r="C416" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A417" t="s">
+        <v>6</v>
+      </c>
+      <c r="B417" t="s">
         <v>315</v>
       </c>
-      <c r="C415" t="s">
+      <c r="C417" t="s">
         <v>442</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" autoFilter="0"/>
-  <autoFilter ref="A1:C415" xr:uid="{FA20B5A7-A3E2-3F42-944A-67FC92CE6A4B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A161:B281">
-    <sortCondition ref="B281"/>
+  <autoFilter ref="A1:C417" xr:uid="{FA20B5A7-A3E2-3F42-944A-67FC92CE6A4B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A161:B283">
+    <sortCondition ref="B283"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>